<commit_message>
update history contract data in db
</commit_message>
<xml_diff>
--- a/steel/data/mid-stream/线材/线材产量.xlsx
+++ b/steel/data/mid-stream/线材/线材产量.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Repository\Projects\ffa\data\钢铁产业链\中游数据\线材\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Document\Project\ffa\steel\data\mid-stream\线材\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66728737-21D1-4202-952E-8A89B5D9F074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C542C76-415A-41DF-A977-ED893044551A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="277" windowWidth="38596" windowHeight="20146" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>howard</author>
+    <author>FUDIAN</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{8110B63B-88FD-4414-BA51-1F6516083CB9}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7BC51633-700E-4731-8DFB-21E7300A79FB}">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>yVjpCgZpNvP6Q15hkl7rf+03AqAeYS/mfkHht955K256ylLhRRIVj1AweNyviIE6DQlzE+G5jsl3z/KR+A52VagO5tN68ASF95UK/eLuMnsi6eJ5AR0wgUzfYoi9AVx1W1G2U46st1i0YMKI2eaiX6Qtpwc36Wulw3Lno0KTwtsGz9xtf1qkBgDQwJYWdnv9y3HMwwNk7kucBZbiH0oAMpNFOPv7CXo8C6piYACuLsbjQyyijuY1nuEPAaXNpQ3bSh17bdoKLxkm030v4jrwggnfawOfoNIPR3OI1dbOgL7XFg6rZ/LW7/s5itpcMY7iry6uZ/HVRVG4JAAbSqhsZRquvg9c/Y1oe5a8EIuJ6btFCstDmVhwokTaHaUoaqXYO9znBunasO8LAn2yepLrtDzLSzkpDxZhK5bPDgJWQoAKv8g+kIADKLiHHVSF0S7SKEzWjRsCTEkiRmWkuzIzaGsBDyZgC5todqB6aQ80xx5EDgBnkQ0Mvco0nKPOEyI3JOp/kQxEkie81h/f7pB0iK54VWpGmhQdFLlNmcKrff1vU6olrsfVPQxSYnEGJINepEyAXkypvCulah5SZwLq+K3urPuKcuOumjnD1xk3KHW9LZgHsK+c4vxCL8v67fcwFG7Dz5MyO6kmhUX3hpIubipLtNYznfyRCvN+NZXTHPQWqmHgZqqkrewPC3J8EmNKwOTVTOPEJLND1NpipVcx2Uz2fJGks4fggiUD7FLrDXW75lEkI6t7jChdIfiLNfwErUC/lkCXsgidIXP+yfS9X5EqWCD1l7u8HjHGaIBYz+JctP89QDYbn7oPDna212+j8JoFIomKOEoEUN8kA/FoRGzP91iTvd2132OLb6S588XfuRcgV73vVqHbLnddNs6tuZy+hAOerHolrOsLan7EbsjOi3f8T04tDOUcU2QDowx6a3TBnKg61tuQ2oUJ6iOFGyAuIcxlDTpGuT/K2PvSx3QyXpw8vWHZPdAV28ZWrPtXIhIuOZ7D1ZeZHl/Iez2E</t>
+          <t>yVjpCgZpNvOHlEoAN60+iXcNR8qcjD2afR3U+XlDrUTEX5W5KWYQZl2WlS6znR8JdtRv8fy9hcGzGgX1t8jwbDwAx0EUQZsw3ZWNu8RJYhGO4TcQ9l1JkQHbe3Y9+FG0Tmzb5nAqIClWWKfYkQKr3HY3DNkUELEitQOt11rUEoT9X4LnIF2tNaex6dI52gDp4SoLch2gg8vELIYnQBqOIz3x9XjVjiDINban2s4akm/JSL8ietbFjayzgtNEk42wlkGLX1qoW5xqK02JFPzlDw1cppIS7RNc566c+GAFC5ydVu28CT0+W5gnBpboU8LhEu98Ou/DawfXMyE567WLlUF690lI/fs5giuIUTL1z6ht0oIb3sfZn9siGCjKdvtVGw+BNjxgn9vI0i9dn7eZKS5lGTFFLhWtQaFCHd07en6QBtYmshUl45fzLLf+O9WxuBRP6/7TIaFUxRWFAs5w16vt3t9EkDSRKSt0VC86hHHOXhfQ77sxLvYt54999AqgS17FkczEdiHdyRIW0iHf257Mo50ybxR7T6lAvRM88GtFqDyq0rey3c2ae2R6651f1tfcFes2aj+AzUOvvlDkU6HDVa0ibZwaGKF8aXqmChUNliA5fetRFoSwnlF7+cZ1e6qJAc4274tbJ+D8tMMMHqTSbtAo9irlAHPxgK5SIXu8G7F5P96BTb1nuRHmCAKUALp8GLTDUrOvZGeGEKT/HzGE590O9is+s7AE5USKr7E2CpSXyUluYyajCWxn6yzxCNa0bG9MCdrWadzO98wR7TlP3/MepkGWMpn8nY7eDOvqFdPesemF+YtMzgKSCmHMWaM/d5iEc9cwSgqRcmyHZsN0AmQkTkAYEl6wGzA6vOE8FD7B9TuYkMlgaxO2wkWabQ7EV0eRBEQolXXXO6Y0oaP8w1GK4dPUPsDMN5bY/a1VhIkaliqP1QsIzpaC3+Efk4/826L12aVs+K8qomt6Fm+lyWpKb0M3oT2eRBYHuLsHhjTPwNsdJ1g9rabkPPJ5DJ+G8GobqXh1t18mQ7hnhVU31v2qw8ke+odUEmVd9P77LO4wzFPASy+5LOLa+NahF0z/512VavYi4cxNozRNG7qChxEmX6c/6h50WmPV2CK0pTb0Qt6WJZ9oBW8wEeJYr/3KozxqEmFzcjmxYWx66qVMs9l5XPVnDrt4zCoq72rTrmm5J6XbcoUMKEOah6a7f3+4YGQch6DZ9pOoWbOyG2Fn15aQi5ivrJb4ee5IChqC4lghZUkvpVtaPew11+lO8gamtBMEOxZFPhorEcV7dI3ToeP6ZAmMYJUpAG/vTgjMWatb53G7VfrA1DNP6fR3QKAQc6a7/mKde4VEaJh9kP9Iqbuwwl7QixfbFrKLP6RF3rCAgUjgGgsdIZNlSwQuc22rkQmPqLTGO+F8xidrhgqVDGqVnuO3Um4BmmcDuc8Fd5V+HzIY2mcQ05qPudfMXekVOyjNhAPK1nb2cvp1pxn7f+4D6Ihz</t>
         </r>
       </text>
     </comment>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>指标名称</t>
   </si>
@@ -107,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -244,7 +244,7 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -750,28 +750,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.53125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="str">
         <f>[1]!EM_EDB_N("2010-3-29","N","Columns=Name,Frequency,Unit,Source&amp;Order=2&amp;DateFormat=1&amp;Chart=2&amp;ClearArea=NULL&amp;CellFormat=1&amp;Layout=0")</f>
         <v>宏观数据</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -788,7 +788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -805,7 +805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -822,7 +822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -839,7 +839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>40268</v>
       </c>
@@ -856,7 +856,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>40298</v>
       </c>
@@ -873,7 +873,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>40329</v>
       </c>
@@ -890,7 +890,7 @@
         <v>21.420100000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5">
         <v>40359</v>
       </c>
@@ -907,7 +907,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <v>40390</v>
       </c>
@@ -924,7 +924,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5">
         <v>40421</v>
       </c>
@@ -941,7 +941,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
         <v>40451</v>
       </c>
@@ -958,7 +958,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5">
         <v>40482</v>
       </c>
@@ -975,7 +975,7 @@
         <v>10.881</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="5">
         <v>40512</v>
       </c>
@@ -992,7 +992,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
         <v>40543</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="5">
         <v>40574</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>16.704699999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="5">
         <v>40602</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="5">
         <v>40633</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5">
         <v>40663</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5">
         <v>40694</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="5">
         <v>40724</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="5">
         <v>40755</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5">
         <v>40786</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5">
         <v>40816</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5">
         <v>40847</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5">
         <v>40877</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>17.815799999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="5">
         <v>40908</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="5">
         <v>40939</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>4.6024000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="5">
         <v>40968</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>7.6189999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="5">
         <v>40999</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>8.0236000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="5">
         <v>41029</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>8.9832999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5">
         <v>41060</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>9.8337000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="5">
         <v>41090</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>11.521599999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="5">
         <v>41121</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>11.331200000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="5">
         <v>41152</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>10.9244</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="5">
         <v>41182</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>10.8033</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="5">
         <v>41213</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>11.3957</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="5">
         <v>41243</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>12.159623</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5">
         <v>41274</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>12.042199999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5">
         <v>41333</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>13.713743729999999</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5">
         <v>41364</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>11.87025015</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="5">
         <v>41394</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>10.05587308</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="5">
         <v>41425</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>11.38933982</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="5">
         <v>41455</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>10.862750119999999</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="5">
         <v>41486</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>11.303598089999999</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="5">
         <v>41517</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>11.5947911</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="5">
         <v>41547</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>11.77100132</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="5">
         <v>41578</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>10.14761575</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="5">
         <v>41608</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>9.6094152400000006</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="5">
         <v>41639</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>9.5810078099999991</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="5">
         <v>41698</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>0.81984623000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="5">
         <v>41729</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>1.90693095</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="5">
         <v>41759</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>4.9274283299999997</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="5">
         <v>41790</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>5.0981039800000003</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="5">
         <v>41820</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>5.4487922099999997</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="5">
         <v>41851</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>5.3393853</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="5">
         <v>41882</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>4.9637766000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="5">
         <v>41912</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>4.1181942300000003</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="5">
         <v>41943</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>3.3448540699999998</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="5">
         <v>41973</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>3.1261518399999999</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="5">
         <v>42004</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>3.22618502</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="5">
         <v>42063</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>-4.8425081600000004</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="5">
         <v>42094</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>-2.1968638199999999</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="5">
         <v>42124</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>-1.5379030499999999</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="5">
         <v>42155</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>-1.7581642399999999</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="5">
         <v>42185</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>-2.3016207199999998</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="5">
         <v>42216</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>-3.4106797599999998</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="5">
         <v>42247</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>-3.5247624700000002</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="5">
         <v>42277</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>-3.42253681</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="5">
         <v>42308</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>-3.8673980399999999</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="5">
         <v>42338</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>-4.0999999999999996</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="5">
         <v>42369</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>-4.5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="5">
         <v>42429</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>-10.4</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="5">
         <v>42460</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="5">
         <v>42490</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="5">
         <v>42521</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>-3.8</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="5">
         <v>42551</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>-3.4</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="5">
         <v>42582</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>-3.1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="5">
         <v>42613</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>-2.9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="5">
         <v>42643</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="5">
         <v>42674</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="5">
         <v>42704</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="5">
         <v>42735</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="5">
         <v>42794</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="5">
         <v>42825</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="5">
         <v>42855</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>-3.1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="5">
         <v>42886</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="5">
         <v>42916</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="5">
         <v>42947</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="5">
         <v>42978</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>-3.9</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="5">
         <v>43008</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="5">
         <v>43039</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="5">
         <v>43069</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="5">
         <v>43100</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="5">
         <v>43159</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="5">
         <v>43190</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="5">
         <v>43220</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="5">
         <v>43251</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="5">
         <v>43281</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="5">
         <v>43312</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="5">
         <v>43343</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="5">
         <v>43373</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="5">
         <v>43404</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="5">
         <v>43434</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="5">
         <v>43465</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="5">
         <v>43524</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="5">
         <v>43555</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="5">
         <v>43585</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="5">
         <v>43616</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="5">
         <v>43646</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="5">
         <v>43677</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="5">
         <v>43708</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="5">
         <v>43738</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="5">
         <v>43769</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="5">
         <v>43799</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="5">
         <v>43830</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="5">
         <v>43890</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>-4.9000000000000004</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="5">
         <v>43921</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="5">
         <v>43951</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>-3.1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="5">
         <v>43982</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="5">
         <v>44012</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="5">
         <v>44043</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="5">
         <v>44074</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="5">
         <v>44104</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="5">
         <v>44135</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="5">
         <v>44165</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="5">
         <v>44196</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="5">
         <v>44255</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="5">
         <v>44286</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="5">
         <v>44316</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="5">
         <v>44347</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="5">
         <v>44377</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="5">
         <v>44408</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="5">
         <v>44439</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="5">
         <v>44469</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="5">
         <v>44500</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="5">
         <v>44530</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>-6.9</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="5">
         <v>44561</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>-7.2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="5">
         <v>44620</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>-16.7</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="5">
         <v>44651</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>-16.8</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="5">
         <v>44681</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>-15.9</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="5">
         <v>44712</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>-15.1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="5">
         <v>44742</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>-13.8</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="5">
         <v>44773</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>-13.7</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="5">
         <v>44804</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>-12.3</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="5">
         <v>44834</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>-9.4</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="5">
         <v>44865</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>-8.4</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="5">
         <v>44895</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>-7.7</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="5">
         <v>44926</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>-8.1999999999999993</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="5">
         <v>44985</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A151" s="5">
         <v>45016</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A152" s="5">
         <v>45046</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A153" s="5">
         <v>45077</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A154" s="5">
         <v>45107</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A155" s="5">
         <v>45138</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A156" s="5">
         <v>45169</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A157" s="5">
         <v>45199</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A158" s="5">
         <v>45230</v>
       </c>
@@ -3400,13 +3400,35 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A159" s="5">
+        <v>45260</v>
+      </c>
+      <c r="B159" s="6">
+        <v>11108000</v>
+      </c>
+      <c r="C159" s="6">
+        <v>3.1</v>
+      </c>
+      <c r="D159" s="6">
+        <v>126509000</v>
+      </c>
+      <c r="E159" s="6">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A160" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A161" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A162" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1.update data to 2024-1-19; 2.implement auto-complete data downloading code
</commit_message>
<xml_diff>
--- a/steel/data/mid-stream/线材/线材产量.xlsx
+++ b/steel/data/mid-stream/线材/线材产量.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Document\Project\ffa\steel\data\mid-stream\线材\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Projects\ffa\steel\data\mid-stream\线材\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C542C76-415A-41DF-A977-ED893044551A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64823BF-08F3-45D3-82FB-0151FAD1F0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1837" yWindow="2213" windowWidth="28800" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>FUDIAN</author>
+    <author>howard</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7BC51633-700E-4731-8DFB-21E7300A79FB}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3621EEE2-E6ED-48BF-A57F-ABEED834391F}">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>yVjpCgZpNvOHlEoAN60+iXcNR8qcjD2afR3U+XlDrUTEX5W5KWYQZl2WlS6znR8JdtRv8fy9hcGzGgX1t8jwbDwAx0EUQZsw3ZWNu8RJYhGO4TcQ9l1JkQHbe3Y9+FG0Tmzb5nAqIClWWKfYkQKr3HY3DNkUELEitQOt11rUEoT9X4LnIF2tNaex6dI52gDp4SoLch2gg8vELIYnQBqOIz3x9XjVjiDINban2s4akm/JSL8ietbFjayzgtNEk42wlkGLX1qoW5xqK02JFPzlDw1cppIS7RNc566c+GAFC5ydVu28CT0+W5gnBpboU8LhEu98Ou/DawfXMyE567WLlUF690lI/fs5giuIUTL1z6ht0oIb3sfZn9siGCjKdvtVGw+BNjxgn9vI0i9dn7eZKS5lGTFFLhWtQaFCHd07en6QBtYmshUl45fzLLf+O9WxuBRP6/7TIaFUxRWFAs5w16vt3t9EkDSRKSt0VC86hHHOXhfQ77sxLvYt54999AqgS17FkczEdiHdyRIW0iHf257Mo50ybxR7T6lAvRM88GtFqDyq0rey3c2ae2R6651f1tfcFes2aj+AzUOvvlDkU6HDVa0ibZwaGKF8aXqmChUNliA5fetRFoSwnlF7+cZ1e6qJAc4274tbJ+D8tMMMHqTSbtAo9irlAHPxgK5SIXu8G7F5P96BTb1nuRHmCAKUALp8GLTDUrOvZGeGEKT/HzGE590O9is+s7AE5USKr7E2CpSXyUluYyajCWxn6yzxCNa0bG9MCdrWadzO98wR7TlP3/MepkGWMpn8nY7eDOvqFdPesemF+YtMzgKSCmHMWaM/d5iEc9cwSgqRcmyHZsN0AmQkTkAYEl6wGzA6vOE8FD7B9TuYkMlgaxO2wkWabQ7EV0eRBEQolXXXO6Y0oaP8w1GK4dPUPsDMN5bY/a1VhIkaliqP1QsIzpaC3+Efk4/826L12aVs+K8qomt6Fm+lyWpKb0M3oT2eRBYHuLsHhjTPwNsdJ1g9rabkPPJ5DJ+G8GobqXh1t18mQ7hnhVU31v2qw8ke+odUEmVd9P77LO4wzFPASy+5LOLa+NahF0z/512VavYi4cxNozRNG7qChxEmX6c/6h50WmPV2CK0pTb0Qt6WJZ9oBW8wEeJYr/3KozxqEmFzcjmxYWx66qVMs9l5XPVnDrt4zCoq72rTrmm5J6XbcoUMKEOah6a7f3+4YGQch6DZ9pOoWbOyG2Fn15aQi5ivrJb4ee5IChqC4lghZUkvpVtaPew11+lO8gamtBMEOxZFPhorEcV7dI3ToeP6ZAmMYJUpAG/vTgjMWatb53G7VfrA1DNP6fR3QKAQc6a7/mKde4VEaJh9kP9Iqbuwwl7QixfbFrKLP6RF3rCAgUjgGgsdIZNlSwQuc22rkQmPqLTGO+F8xidrhgqVDGqVnuO3Um4BmmcDuc8Fd5V+HzIY2mcQ05qPudfMXekVOyjNhAPK1nb2cvp1pxn7f+4D6Ihz</t>
+          <t>yVjpCgZpNvMUSeU5qcmzKp2wgSpJ+89366KKsey93YFOUjSgqoOUXXab+w7ncG+mCX8YCa6x35GPgPCmi/6jEjF3ET7Ub+ZdmBGj8hfCnyrsKssJ7f86QEb8Xz9bPX20sVW5M9wvz4nxjje18gaXmvOyVB+sA0jJ8+8FKOqbDarmS6/r0831z55eKXRv6NT2+FIncFo6rnVvKkv1LGBD/CsVEERfAYfTbn2vlvbgRpaIWgB3K4wViSOezCeYrs2supeLUkbW9H/ZzYVOIlzV5a0TEvGM3QJ9yE6GTfYFnUgmg6+jrY6oHTUnf/t3dKurbqlMvpdDJm0gPvzpWFOUz9/yyjYNl1iIvBfbIu8vVkx78pfhoTBkVcAEQi62qO1n+ObWrrEEeFemnDONA5LP5LVUezg6TJbDbxr/vgm7zxNjHne6J02Dh2JXt2Z4B6+Vt7E1K5A9lWFGhZJ4Qg1RpMVr6r353XZESitIRksQldKDxsO7w5yz8++4xySUSbysNlc5RwzufSmEOC4f9YlFnzfEmDxwmzMAezogySIYxZtEhanc5OjSIKSuMyexSL+yb4ho8lZeNNSgMjoHxuaL77EB51k5iNTb9q7DXg9UzVgrtGt3iZAeSId6p5FpV2bYbci/BJp1K1dPqOjdscetsa+klX6gHcRGjb/noaJ73ag2maQ25q+WnAoZGXQt1F1FaWCdQSiqbbvfKZW6GRspXMMulZoRYFNk9uemLhzTpdlqAmNR/6rQNu0oFLYpHO8eZPU3XmC0OhfMNe6XL/8kPYHGDdvrYHTDnVYP8iSe/09ALyfsx5Eo70ADlna6lMYyMuBoFZ1ncOHFlrkQCC+3JB8Zldsk81QcuclYTStTI2+aNcuTQ6R1Qsuc2BQkptU5NBjvRaqqh+XCPb8P1xYuVFrh1nwVbpXBbWVE8QYefprqt8s+4uCk5a56k7MomMG9I8sX010dc1NBIK98/CFMoy9VYKFTKsAc1Nx+zM0kUMUXbQ9jDKZBxbRoVwE7oarN</t>
         </r>
       </text>
     </comment>
@@ -750,28 +750,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="E162" sqref="E162"/>
+      <selection activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>[1]!EM_EDB_N("2010-3-29","N","Columns=Name,Frequency,Unit,Source&amp;Order=2&amp;DateFormat=1&amp;Chart=2&amp;ClearArea=NULL&amp;CellFormat=1&amp;Layout=0")</f>
         <v>宏观数据</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -788,7 +788,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -805,7 +805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -822,7 +822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -839,7 +839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>40268</v>
       </c>
@@ -856,7 +856,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>40298</v>
       </c>
@@ -873,7 +873,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>40329</v>
       </c>
@@ -890,7 +890,7 @@
         <v>21.420100000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>40359</v>
       </c>
@@ -907,7 +907,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>40390</v>
       </c>
@@ -924,7 +924,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>40421</v>
       </c>
@@ -941,7 +941,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>40451</v>
       </c>
@@ -958,7 +958,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>40482</v>
       </c>
@@ -975,7 +975,7 @@
         <v>10.881</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>40512</v>
       </c>
@@ -992,7 +992,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>40543</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>40574</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>16.704699999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>40602</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>40633</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>40663</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>40694</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>40724</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>40755</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>40786</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>40816</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>40847</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>40877</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>17.815799999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>40908</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>40939</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>4.6024000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>40968</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>7.6189999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>40999</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>8.0236000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>41029</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>8.9832999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>41060</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>9.8337000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>41090</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>11.521599999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>41121</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>11.331200000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>41152</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>10.9244</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>41182</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>10.8033</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>41213</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>11.3957</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>41243</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>12.159623</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>41274</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>12.042199999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>41333</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>13.713743729999999</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>41364</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>11.87025015</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41394</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>10.05587308</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>41425</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>11.38933982</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>41455</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>10.862750119999999</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>41486</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>11.303598089999999</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>41517</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>11.5947911</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>41547</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>11.77100132</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>41578</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>10.14761575</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>41608</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>9.6094152400000006</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>41639</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>9.5810078099999991</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>41698</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>0.81984623000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>41729</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>1.90693095</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>41759</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>4.9274283299999997</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>41790</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>5.0981039800000003</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>41820</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>5.4487922099999997</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>41851</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>5.3393853</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>41882</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>4.9637766000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>41912</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>4.1181942300000003</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>41943</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>3.3448540699999998</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>41973</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>3.1261518399999999</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>42004</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>3.22618502</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>42063</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>-4.8425081600000004</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>42094</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>-2.1968638199999999</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>42124</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>-1.5379030499999999</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>42155</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>-1.7581642399999999</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>42185</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>-2.3016207199999998</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>42216</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>-3.4106797599999998</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>42247</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>-3.5247624700000002</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>42277</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>-3.42253681</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>42308</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>-3.8673980399999999</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>42338</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>-4.0999999999999996</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>42369</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>-4.5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>42429</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>-10.4</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>42460</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>42490</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>42521</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>-3.8</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>42551</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>-3.4</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>42582</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>-3.1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>42613</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>-2.9</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>42643</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>42674</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>42704</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>42735</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>42794</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>42825</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>42855</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>-3.1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>42886</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>42916</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>42947</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>42978</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>-3.9</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>43008</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>43039</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>43069</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>43100</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>43159</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>43190</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>43220</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>43251</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>43281</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>43312</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>43343</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>43373</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="5">
         <v>43404</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5">
         <v>43434</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <v>43465</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
         <v>43524</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="5">
         <v>43555</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="5">
         <v>43585</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="5">
         <v>43616</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="5">
         <v>43646</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="5">
         <v>43677</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="5">
         <v>43708</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="5">
         <v>43738</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="5">
         <v>43769</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="5">
         <v>43799</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="5">
         <v>43830</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="5">
         <v>43890</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>-4.9000000000000004</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="5">
         <v>43921</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="5">
         <v>43951</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>-3.1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="5">
         <v>43982</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="5">
         <v>44012</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="5">
         <v>44043</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="5">
         <v>44074</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="5">
         <v>44104</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="5">
         <v>44135</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="5">
         <v>44165</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="5">
         <v>44196</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="5">
         <v>44255</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5">
         <v>44286</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="5">
         <v>44316</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="5">
         <v>44347</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5">
         <v>44377</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5">
         <v>44408</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="5">
         <v>44439</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="5">
         <v>44469</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>-2.2999999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5">
         <v>44500</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>-4.8</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="5">
         <v>44530</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>-6.9</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="5">
         <v>44561</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>-7.2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="5">
         <v>44620</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>-16.7</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="5">
         <v>44651</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>-16.8</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5">
         <v>44681</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>-15.9</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="5">
         <v>44712</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>-15.1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5">
         <v>44742</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>-13.8</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="5">
         <v>44773</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>-13.7</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="5">
         <v>44804</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>-12.3</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="5">
         <v>44834</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>-9.4</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="5">
         <v>44865</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>-8.4</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="5">
         <v>44895</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>-7.7</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="5">
         <v>44926</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>-8.1999999999999993</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="5">
         <v>44985</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="5">
         <v>45016</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="5">
         <v>45046</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="5">
         <v>45077</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="5">
         <v>45107</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="5">
         <v>45138</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="5">
         <v>45169</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="5">
         <v>45199</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="5">
         <v>45230</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>-0.9</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="5">
         <v>45260</v>
       </c>
@@ -3417,18 +3417,35 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A160" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="5">
+        <v>45291</v>
+      </c>
+      <c r="B160" s="6">
+        <v>10833000</v>
+      </c>
+      <c r="C160" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="D160" s="6">
+        <v>137351000</v>
+      </c>
+      <c r="E160" s="6">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>